<commit_message>
Include scaling inventory for India from Venkataraman et al., 2014 and 2018. Added associated invenotry files, mapping file, and changes to the Makefile and F1.inventory_scaling file.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Africa_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Africa_scaling_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE14B9-1B56-6B4D-80B2-92F6B5DC13C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0DC194-CB72-6A4F-B04C-43C9D6E9449F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="2520" windowWidth="29620" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="6940" windowWidth="29620" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>iso</t>
   </si>
@@ -1475,13 +1475,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J161"/>
+  <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1621,7 +1621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>90</v>
       </c>
@@ -1633,6 +1633,12 @@
       </c>
       <c r="D8" s="7" t="s">
         <v>14</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1712,236 +1718,229 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="E14" s="11" t="s">
+    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F15" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="E15" s="21" t="s">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F16" s="31" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="E16" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E17" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E18" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E20" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="F19" s="30"/>
-    </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E20" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="D22"/>
-      <c r="E22" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="29"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="D23"/>
+      <c r="E23" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="D24"/>
-      <c r="E24" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="29"/>
     </row>
     <row r="25" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="D25"/>
+      <c r="E25" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="29"/>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="D26"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E27" s="25" t="s">
+    </row>
+    <row r="27" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+      <c r="D27"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E28" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E29" s="12" t="s">
+      <c r="F28" s="29"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E30" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30" s="8"/>
+      <c r="F30" s="30"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
       <c r="D31"/>
       <c r="E31"/>
+      <c r="F31" s="8"/>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="D32"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E33" s="9" t="s">
+    <row r="33" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E34" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F34" s="30"/>
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E35" s="8"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-    </row>
-    <row r="37" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E36" s="8"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="D37"/>
-      <c r="E37" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="30"/>
-    </row>
-    <row r="38" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E37"/>
+    </row>
+    <row r="38" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="D38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E39" s="19" t="s">
+      <c r="E38" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="30"/>
+    </row>
+    <row r="39" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+    </row>
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E40" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="F39" s="30"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E40" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="F40" s="30"/>
       <c r="J40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E41" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F41" s="30"/>
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="30"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E43" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F42" s="30"/>
-    </row>
-    <row r="43" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43"/>
-      <c r="D43"/>
-      <c r="E43" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="D44"/>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="30"/>
+    </row>
+    <row r="45" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="D45"/>
+      <c r="E45" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="31"/>
-    </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45"/>
-      <c r="E45" s="16" t="s">
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46"/>
+      <c r="E46" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="30"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46"/>
-      <c r="D46"/>
-      <c r="E46" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="F46" s="30"/>
+      <c r="J46" s="8"/>
     </row>
     <row r="47" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="D47"/>
-      <c r="E47" s="18" t="s">
-        <v>41</v>
+      <c r="E47" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="D48"/>
-      <c r="E48" s="13" t="s">
-        <v>28</v>
+      <c r="E48" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="F48" s="30"/>
     </row>
@@ -1949,188 +1948,187 @@
       <c r="A49"/>
       <c r="D49"/>
       <c r="E49" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F49" s="30"/>
     </row>
-    <row r="50" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="D50"/>
-      <c r="E50"/>
+      <c r="E50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="D51"/>
-    </row>
-    <row r="52" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E52" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F52" s="30"/>
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="D52"/>
     </row>
     <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E53" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E54" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="30"/>
+    </row>
+    <row r="55" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E55" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F54" s="30"/>
-    </row>
-    <row r="55" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E55" s="13" t="s">
+      <c r="F55" s="30"/>
+    </row>
+    <row r="56" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E56" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F55" s="30"/>
-    </row>
-    <row r="56" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56"/>
-      <c r="D56"/>
-      <c r="E56" s="13" t="s">
+      <c r="F56" s="30"/>
+    </row>
+    <row r="57" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="D57"/>
+      <c r="E57" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F56" s="30"/>
-    </row>
-    <row r="57" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E57" s="13" t="s">
+      <c r="F57" s="30"/>
+    </row>
+    <row r="58" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E58" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F57" s="30"/>
-      <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58"/>
-      <c r="D58"/>
-      <c r="E58" s="13" t="s">
+      <c r="F58" s="30"/>
+      <c r="J58" s="8"/>
+    </row>
+    <row r="59" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="D59"/>
+      <c r="E59" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F58" s="30"/>
-    </row>
-    <row r="60" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60"/>
-      <c r="D60"/>
-      <c r="E60"/>
+      <c r="F59" s="30"/>
     </row>
     <row r="61" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="D61"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="D62"/>
-      <c r="E62" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F62" s="30"/>
+      <c r="E62"/>
     </row>
     <row r="63" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="D63"/>
-      <c r="E63" s="15" t="s">
+      <c r="E63" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="30"/>
+    </row>
+    <row r="64" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+      <c r="D64"/>
+      <c r="E64" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F63" s="30"/>
-    </row>
-    <row r="64" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E64" s="15" t="s">
+      <c r="F64" s="30"/>
+    </row>
+    <row r="65" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E65" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F64" s="30"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J65" s="8"/>
-    </row>
-    <row r="66" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E66" s="14" t="s">
+      <c r="F65" s="30"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J66" s="8"/>
+    </row>
+    <row r="67" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E67" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F66" s="30"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F67" s="30"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69"/>
-      <c r="D69"/>
-      <c r="E69" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F69" s="31"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E69" s="8"/>
     </row>
     <row r="70" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="D70"/>
       <c r="E70" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F70" s="31"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71"/>
+      <c r="D71"/>
+      <c r="E71" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F70" s="31"/>
-    </row>
-    <row r="71" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E71" s="31" t="s">
+      <c r="F71" s="31"/>
+    </row>
+    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E72" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F71" s="31"/>
-    </row>
-    <row r="72" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-    </row>
-    <row r="73" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
+      <c r="F72" s="31"/>
+    </row>
+    <row r="73" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73"/>
+      <c r="D73"/>
+      <c r="E73"/>
     </row>
     <row r="74" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E74" s="22" t="s">
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+    </row>
+    <row r="75" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E75" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F74" s="30"/>
-    </row>
-    <row r="75" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75"/>
-      <c r="D75"/>
-      <c r="E75" s="22" t="s">
+      <c r="F75" s="30"/>
+    </row>
+    <row r="76" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76"/>
+      <c r="D76"/>
+      <c r="E76" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F75" s="30"/>
-    </row>
-    <row r="76" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E76" s="22" t="s">
+      <c r="F76" s="30"/>
+    </row>
+    <row r="77" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E77" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F76" s="30"/>
-    </row>
-    <row r="77" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77"/>
-      <c r="D77"/>
-      <c r="E77" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="F77" s="30"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
     </row>
     <row r="78" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78"/>
       <c r="D78"/>
-      <c r="E78" s="22"/>
+      <c r="E78" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="F78" s="30"/>
       <c r="G78"/>
       <c r="H78"/>
@@ -2139,58 +2137,62 @@
     <row r="79" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79"/>
       <c r="D79"/>
-      <c r="E79" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F79" s="31"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="30"/>
       <c r="G79"/>
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J80" s="8"/>
+    <row r="80" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80"/>
+      <c r="D80"/>
+      <c r="E80" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F80" s="31"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J81" s="8"/>
     </row>
-    <row r="82" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82"/>
-      <c r="D82"/>
-      <c r="E82" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F82" s="30"/>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J82" s="8"/>
     </row>
     <row r="83" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A83"/>
       <c r="D83"/>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F83" s="30"/>
+    </row>
+    <row r="84" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84"/>
+      <c r="D84"/>
+      <c r="E84" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F83" s="30"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-    </row>
-    <row r="85" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85"/>
-      <c r="D85"/>
-      <c r="E85" s="24" t="s">
+      <c r="F84" s="30"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+    </row>
+    <row r="86" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86"/>
+      <c r="D86"/>
+      <c r="E86" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F85" s="30"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-    </row>
-    <row r="87" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87"/>
-      <c r="D87"/>
-      <c r="E87"/>
+      <c r="F86" s="30"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
     </row>
     <row r="88" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88"/>
@@ -2201,45 +2203,45 @@
       <c r="A89"/>
       <c r="D89"/>
       <c r="E89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-    </row>
-    <row r="91" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91"/>
-      <c r="D91"/>
-      <c r="E91"/>
-      <c r="G91"/>
-      <c r="H91"/>
-      <c r="I91"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-    </row>
-    <row r="93" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93"/>
-      <c r="D93"/>
-      <c r="E93"/>
+    </row>
+    <row r="90" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+    </row>
+    <row r="92" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
     </row>
     <row r="94" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94"/>
       <c r="D94"/>
       <c r="E94"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J95" s="8"/>
-    </row>
-    <row r="96" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96"/>
-      <c r="D96"/>
-      <c r="E96"/>
+    <row r="95" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J96" s="8"/>
     </row>
     <row r="97" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97"/>
@@ -2255,9 +2257,6 @@
       <c r="A99"/>
       <c r="D99"/>
       <c r="E99"/>
-      <c r="G99"/>
-      <c r="H99"/>
-      <c r="I99"/>
     </row>
     <row r="100" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100"/>
@@ -2275,16 +2274,18 @@
       <c r="H101"/>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
+    <row r="102" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
-      <c r="J103" s="8"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G104" s="8"/>
@@ -2292,10 +2293,11 @@
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
     </row>
-    <row r="105" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105"/>
-      <c r="D105"/>
-      <c r="E105"/>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
     </row>
     <row r="106" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106"/>
@@ -2312,8 +2314,10 @@
       <c r="D108"/>
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J109" s="8"/>
+    <row r="109" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109"/>
+      <c r="D109"/>
+      <c r="E109"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J110" s="8"/>
@@ -2322,9 +2326,6 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
       <c r="J112" s="8"/>
     </row>
     <row r="113" spans="7:10" x14ac:dyDescent="0.2">
@@ -2334,6 +2335,9 @@
       <c r="J113" s="8"/>
     </row>
     <row r="114" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+      <c r="I114" s="8"/>
       <c r="J114" s="8"/>
     </row>
     <row r="115" spans="7:10" x14ac:dyDescent="0.2">
@@ -2354,11 +2358,11 @@
     <row r="120" spans="7:10" x14ac:dyDescent="0.2">
       <c r="J120" s="8"/>
     </row>
-    <row r="125" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J125" s="8"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J129" s="8"/>
+    <row r="121" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="J121" s="8"/>
+    </row>
+    <row r="126" spans="7:10" x14ac:dyDescent="0.2">
+      <c r="J126" s="8"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J130" s="8"/>
@@ -2369,24 +2373,24 @@
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J132" s="8"/>
     </row>
-    <row r="133" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A133"/>
-      <c r="D133"/>
-      <c r="E133"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J134" s="8"/>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J133" s="8"/>
+    </row>
+    <row r="134" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134"/>
+      <c r="D134"/>
+      <c r="E134"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J135" s="8"/>
     </row>
-    <row r="136" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136"/>
-      <c r="D136"/>
-      <c r="E136"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J137" s="8"/>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J136" s="8"/>
+    </row>
+    <row r="137" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137"/>
+      <c r="D137"/>
+      <c r="E137"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J138" s="8"/>
@@ -2394,13 +2398,13 @@
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J139" s="8"/>
     </row>
-    <row r="140" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A140"/>
-      <c r="D140"/>
-      <c r="E140"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J141" s="8"/>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J140" s="8"/>
+    </row>
+    <row r="141" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141"/>
+      <c r="D141"/>
+      <c r="E141"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J142" s="8"/>
@@ -2411,13 +2415,13 @@
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J144" s="8"/>
     </row>
-    <row r="145" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145"/>
-      <c r="D145"/>
-      <c r="E145"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J146" s="8"/>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J145" s="8"/>
+    </row>
+    <row r="146" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146"/>
+      <c r="D146"/>
+      <c r="E146"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J147" s="8"/>
@@ -2428,13 +2432,13 @@
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J149" s="8"/>
     </row>
-    <row r="150" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A150"/>
-      <c r="D150"/>
-      <c r="E150"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J151" s="8"/>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J150" s="8"/>
+    </row>
+    <row r="151" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A151"/>
+      <c r="D151"/>
+      <c r="E151"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J152" s="8"/>
@@ -2442,30 +2446,33 @@
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J153" s="8"/>
     </row>
-    <row r="154" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A154"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154"/>
-      <c r="E154"/>
-      <c r="F154" s="8"/>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J154" s="8"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="8"/>
+      <c r="D155"/>
+      <c r="E155"/>
+      <c r="F155" s="8"/>
       <c r="J155" s="8"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J158" s="8"/>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J156" s="8"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H160" s="8"/>
       <c r="J160" s="8"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H161" s="8"/>
       <c r="J161" s="8"/>
+    </row>
+    <row r="162" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="J162" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J1">

</xml_diff>

<commit_message>
Updates to Africa DICE inventory scaling procedure 1. Added DICE inventory years for 2006 (now scaled to 2006 and 2013) 2. Changed max scaling factor from 100 to 1000 (to better capture residential light oil use) 3. Added scaling for BC and OC 4. Fixed mapping file
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Africa_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Africa_scaling_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0DC194-CB72-6A4F-B04C-43C9D6E9449F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77C55AE-F64D-CC44-9470-E648D54E4F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="6940" windowWidth="29620" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="2880" windowWidth="25680" windowHeight="15120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t>iso</t>
   </si>
@@ -77,9 +77,6 @@
     <t>ceds_sector</t>
   </si>
   <si>
-    <t>RCO</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -309,6 +306,15 @@
   </si>
   <si>
     <t>motorcycles</t>
+  </si>
+  <si>
+    <t>residential</t>
+  </si>
+  <si>
+    <t>ben</t>
+  </si>
+  <si>
+    <t>residential emissions spike if same scaling factor is applied before 2013. Res emissions therefore may be under-predicted, but will be over-predicted otherwise</t>
   </si>
 </sst>
 </file>
@@ -1475,21 +1481,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8:F8"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="3" width="18.1640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="8" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
@@ -1499,10 +1506,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
@@ -1511,269 +1518,268 @@
         <v>13</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="7"/>
       <c r="G4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="E9" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>14</v>
+        <v>83</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="7"/>
       <c r="G12" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
         <v>87</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="G13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E15" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="E16" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E17" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E18" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E19" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E20" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E21" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E22" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="30"/>
     </row>
@@ -1781,123 +1787,153 @@
       <c r="A23"/>
       <c r="D23"/>
       <c r="E23" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="D24"/>
-    </row>
-    <row r="25" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="D25"/>
-      <c r="E25" s="27" t="s">
-        <v>53</v>
+      <c r="E24" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E25" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="F25" s="29"/>
     </row>
-    <row r="26" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="D27"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E28" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="29"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E29" s="8"/>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28"/>
+      <c r="D28"/>
+      <c r="E28" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="30"/>
+    </row>
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E29" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="J29" s="8"/>
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E30" s="12" t="s">
-        <v>21</v>
+      <c r="E30" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="F30" s="30"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31" s="8"/>
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E31" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="30"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E32" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="D33"/>
-      <c r="E33"/>
-    </row>
-    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="30"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E33" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="D34"/>
+      <c r="E34" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35"/>
+      <c r="E35" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="30"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E36" s="8"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36"/>
+      <c r="D36"/>
+      <c r="E36" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="D37"/>
-      <c r="E37"/>
+      <c r="E37" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="D38"/>
-      <c r="E38" s="30" t="s">
-        <v>64</v>
+      <c r="E38" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="F38" s="30"/>
     </row>
-    <row r="39" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="D39"/>
-      <c r="E39"/>
+      <c r="E39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E40" s="19" t="s">
-        <v>42</v>
+      <c r="E40" s="28" t="s">
+        <v>53</v>
       </c>
       <c r="F40" s="30"/>
-      <c r="J40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E41" s="13" t="s">
-        <v>24</v>
+      <c r="E41" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="F41" s="30"/>
-      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E42" s="13" t="s">
-        <v>23</v>
+      <c r="E42" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="F42" s="30"/>
-      <c r="J42" s="8"/>
     </row>
     <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E43" s="20" t="s">
-        <v>43</v>
+      <c r="E43" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="F43" s="30"/>
     </row>
@@ -1905,414 +1941,331 @@
       <c r="A44"/>
       <c r="D44"/>
       <c r="E44" s="13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F44" s="30"/>
     </row>
-    <row r="45" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45"/>
-      <c r="D45"/>
-      <c r="E45" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="31"/>
-    </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="E45" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="30"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
       <c r="D46"/>
-      <c r="E46" s="16" t="s">
-        <v>39</v>
+      <c r="E46" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="F46" s="30"/>
-      <c r="J46" s="8"/>
     </row>
     <row r="47" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="D47"/>
-      <c r="E47" s="17" t="s">
-        <v>40</v>
+      <c r="E47" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="D48"/>
-      <c r="E48" s="18" t="s">
-        <v>41</v>
+      <c r="E48" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="F48" s="30"/>
     </row>
-    <row r="49" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49"/>
-      <c r="D49"/>
-      <c r="E49" s="13" t="s">
-        <v>28</v>
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E49" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="F49" s="30"/>
     </row>
-    <row r="50" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50"/>
-      <c r="D50"/>
-      <c r="E50" s="13" t="s">
-        <v>32</v>
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E50" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="F50" s="30"/>
-    </row>
-    <row r="51" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="D51"/>
-      <c r="E51"/>
-    </row>
-    <row r="52" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="31"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="D52"/>
-    </row>
-    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E53" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" s="30"/>
-    </row>
-    <row r="54" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E54" s="28" t="s">
-        <v>55</v>
+      <c r="E52" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E53" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" s="31"/>
+    </row>
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E54" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="F54" s="30"/>
     </row>
-    <row r="55" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E55" s="28" t="s">
-        <v>56</v>
+    <row r="55" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="D55"/>
+      <c r="E55" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="F55" s="30"/>
     </row>
-    <row r="56" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E56" s="13" t="s">
-        <v>22</v>
+    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="E56" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="F56" s="30"/>
     </row>
-    <row r="57" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="D57"/>
-      <c r="E57" s="13" t="s">
-        <v>29</v>
+      <c r="E57" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F57" s="30"/>
-    </row>
-    <row r="58" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E58" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="30"/>
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="D58"/>
+      <c r="E58" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" s="31"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="D59"/>
-      <c r="E59" s="13" t="s">
-        <v>31</v>
+      <c r="E59" s="30" t="s">
+        <v>59</v>
       </c>
       <c r="F59" s="30"/>
     </row>
-    <row r="61" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60"/>
+      <c r="D60"/>
+      <c r="E60" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" s="30"/>
+    </row>
+    <row r="61" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="D61"/>
-      <c r="E61"/>
-    </row>
-    <row r="62" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-    </row>
-    <row r="63" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="E61" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" s="30"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+    </row>
+    <row r="63" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="D63"/>
-      <c r="E63" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F63" s="30"/>
-    </row>
-    <row r="64" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="E63"/>
+    </row>
+    <row r="64" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="D64"/>
-      <c r="E64" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F64" s="30"/>
-    </row>
-    <row r="65" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E65" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="30"/>
+      <c r="E64"/>
+    </row>
+    <row r="65" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J66" s="8"/>
-    </row>
-    <row r="67" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E67" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F67" s="30"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+    </row>
+    <row r="67" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E69" s="8"/>
-    </row>
-    <row r="70" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+    </row>
+    <row r="70" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="D70"/>
-      <c r="E70" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F70" s="31"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71"/>
-      <c r="D71"/>
-      <c r="E71" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" s="31"/>
-    </row>
-    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E72" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F72" s="31"/>
+      <c r="E70"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J71" s="8"/>
+    </row>
+    <row r="72" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72"/>
+      <c r="D72"/>
+      <c r="E72"/>
     </row>
     <row r="73" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="D73"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-    </row>
-    <row r="75" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E75" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F75" s="30"/>
-    </row>
-    <row r="76" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+    </row>
+    <row r="75" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76"/>
       <c r="D76"/>
-      <c r="E76" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F76" s="30"/>
-    </row>
-    <row r="77" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="E77" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F77" s="30"/>
-    </row>
-    <row r="78" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78"/>
-      <c r="D78"/>
-      <c r="E78" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F78" s="30"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79"/>
-      <c r="D79"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="30"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
-    </row>
-    <row r="80" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80"/>
-      <c r="D80"/>
-      <c r="E80" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F80" s="31"/>
-      <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J81" s="8"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J82" s="8"/>
-    </row>
-    <row r="83" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="E76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+    </row>
+    <row r="81" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83"/>
       <c r="D83"/>
-      <c r="E83" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F83" s="30"/>
-    </row>
-    <row r="84" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84"/>
       <c r="D84"/>
-      <c r="E84" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F84" s="30"/>
+      <c r="E84"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
       <c r="J85" s="8"/>
     </row>
-    <row r="86" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86"/>
-      <c r="D86"/>
-      <c r="E86" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F86" s="30"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-    </row>
-    <row r="88" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-    </row>
-    <row r="89" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89"/>
-      <c r="D89"/>
-      <c r="E89"/>
-    </row>
-    <row r="90" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="G90"/>
-      <c r="H90"/>
-      <c r="I90"/>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J86" s="8"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J87" s="8"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J90" s="8"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-    </row>
-    <row r="92" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92"/>
-      <c r="D92"/>
-      <c r="E92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
+      <c r="J91" s="8"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J92" s="8"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-    </row>
-    <row r="94" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94"/>
-      <c r="D94"/>
-      <c r="E94"/>
-    </row>
-    <row r="95" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95"/>
-      <c r="D95"/>
-      <c r="E95"/>
+      <c r="J93" s="8"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J94" s="8"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J96" s="8"/>
     </row>
-    <row r="97" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97"/>
-      <c r="D97"/>
-      <c r="E97"/>
-    </row>
-    <row r="98" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98"/>
-      <c r="D98"/>
-      <c r="E98"/>
-    </row>
-    <row r="99" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99"/>
-      <c r="D99"/>
-      <c r="E99"/>
-    </row>
-    <row r="100" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100"/>
-      <c r="D100"/>
-      <c r="E100"/>
-      <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
-    </row>
-    <row r="101" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101"/>
-      <c r="D101"/>
-      <c r="E101"/>
-      <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
-    </row>
-    <row r="102" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102"/>
-      <c r="D102"/>
-      <c r="E102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="8"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="8"/>
-      <c r="J104" s="8"/>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J101" s="8"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
-      <c r="I105" s="8"/>
       <c r="J105" s="8"/>
     </row>
-    <row r="106" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106"/>
-      <c r="D106"/>
-      <c r="E106"/>
-    </row>
-    <row r="107" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107"/>
-      <c r="D107"/>
-      <c r="E107"/>
-    </row>
-    <row r="108" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108"/>
-      <c r="D108"/>
-      <c r="E108"/>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J106" s="8"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J107" s="8"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J108" s="8"/>
     </row>
     <row r="109" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109"/>
@@ -2325,154 +2278,92 @@
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J111" s="8"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J112" s="8"/>
-    </row>
-    <row r="113" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
-      <c r="I113" s="8"/>
+    <row r="112" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112"/>
+      <c r="D112"/>
+      <c r="E112"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J113" s="8"/>
     </row>
-    <row r="114" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
-      <c r="I114" s="8"/>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J114" s="8"/>
     </row>
-    <row r="115" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J115" s="8"/>
     </row>
-    <row r="116" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J116" s="8"/>
-    </row>
-    <row r="117" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116"/>
+      <c r="D116"/>
+      <c r="E116"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J117" s="8"/>
     </row>
-    <row r="118" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J118" s="8"/>
     </row>
-    <row r="119" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J119" s="8"/>
     </row>
-    <row r="120" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J120" s="8"/>
     </row>
-    <row r="121" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J121" s="8"/>
-    </row>
-    <row r="126" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J126" s="8"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121"/>
+      <c r="D121"/>
+      <c r="E121"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J122" s="8"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J123" s="8"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J124" s="8"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J125" s="8"/>
+    </row>
+    <row r="126" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126"/>
+      <c r="D126"/>
+      <c r="E126"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J127" s="8"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J128" s="8"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J129" s="8"/>
+    </row>
+    <row r="130" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130" s="8"/>
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J131" s="8"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J132" s="8"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J133" s="8"/>
-    </row>
-    <row r="134" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134"/>
-      <c r="D134"/>
-      <c r="E134"/>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J134" s="8"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H136" s="8"/>
       <c r="J136" s="8"/>
     </row>
-    <row r="137" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A137"/>
-      <c r="D137"/>
-      <c r="E137"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J138" s="8"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J139" s="8"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J140" s="8"/>
-    </row>
-    <row r="141" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141"/>
-      <c r="D141"/>
-      <c r="E141"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J142" s="8"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J143" s="8"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J144" s="8"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J145" s="8"/>
-    </row>
-    <row r="146" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146"/>
-      <c r="D146"/>
-      <c r="E146"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J147" s="8"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J148" s="8"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J149" s="8"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J150" s="8"/>
-    </row>
-    <row r="151" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A151"/>
-      <c r="D151"/>
-      <c r="E151"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J152" s="8"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J153" s="8"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J154" s="8"/>
-    </row>
-    <row r="155" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155"/>
-      <c r="E155"/>
-      <c r="F155" s="8"/>
-      <c r="J155" s="8"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J156" s="8"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J159" s="8"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J160" s="8"/>
-    </row>
-    <row r="161" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H161" s="8"/>
-      <c r="J161" s="8"/>
-    </row>
-    <row r="162" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="J162" s="8"/>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J137" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J1">
@@ -2500,6 +2391,8 @@
   <cols>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2510,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>9</v>
@@ -2562,13 +2455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.83203125" style="8"/>
+    <col min="3" max="3" width="12.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2579,7 +2474,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -2600,32 +2495,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>2006</v>
+      </c>
+      <c r="E2">
+        <v>2018</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="G2">
+        <v>2006</v>
+      </c>
+      <c r="H2">
         <v>2013</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="5"/>
+      <c r="I2" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>